<commit_message>
Stetson art, sizes fix
</commit_message>
<xml_diff>
--- a/Excel/Stetson/2022.02.08/24.02.2022 STETSON — техничка.xlsx
+++ b/Excel/Stetson/2022.02.08/24.02.2022 STETSON — техничка.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BUH\Documents\HatsAndCaps\Excel\Stetson\2022.02.08\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A345B2-EA19-4BB6-A9CB-65921E350F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D37CA2-B7FA-49EB-BF19-E4A41BC3E668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DCE1A16A-D28B-4C15-8FE6-3AA1412CC8DB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="252">
   <si>
     <t>Артикул на этикетке</t>
   </si>
@@ -788,6 +788,12 @@
   </si>
   <si>
     <t>Женский</t>
+  </si>
+  <si>
+    <t>темно-бежевый</t>
+  </si>
+  <si>
+    <t>02-654-83</t>
   </si>
 </sst>
 </file>
@@ -795,8 +801,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00\ [$₽-419]"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ [$₽-419]"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -913,13 +919,13 @@
     <xf numFmtId="12" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -955,14 +961,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -997,10 +1003,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1367,7 +1373,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4621213" y="11861800"/>
+          <a:off x="5256667" y="11846832"/>
           <a:ext cx="1778000" cy="965200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4882,9 +4888,9 @@
   </sheetPr>
   <dimension ref="A1:AN112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="98.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5621,7 +5627,7 @@
     </row>
     <row r="8" spans="1:40" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>69</v>
+        <v>251</v>
       </c>
       <c r="B8" s="10" t="str">
         <f t="shared" si="0"/>
@@ -5653,7 +5659,7 @@
         <v>67</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>58</v>
+        <v>250</v>
       </c>
       <c r="M8" s="17" t="s">
         <v>62</v>

</xml_diff>